<commit_message>
updated for single words
</commit_message>
<xml_diff>
--- a/Keyword Map NLP.xlsx
+++ b/Keyword Map NLP.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="146">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="147">
   <si>
     <t xml:space="preserve">Keyword</t>
   </si>
@@ -458,6 +458,9 @@
   </si>
   <si>
     <t xml:space="preserve">rewind</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cabinet</t>
   </si>
 </sst>
 </file>
@@ -565,11 +568,11 @@
   </sheetPr>
   <dimension ref="A1:H1024"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A85" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C151" activeCellId="0" sqref="C151"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A106" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F143" activeCellId="0" sqref="F143"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.46484375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.47265625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="12.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="2" style="0" width="8.7"/>
@@ -4241,7 +4244,32 @@
         <v>0</v>
       </c>
     </row>
-    <row r="142" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="142" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A142" s="0" t="s">
+        <v>146</v>
+      </c>
+      <c r="B142" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="C142" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D142" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E142" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F142" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G142" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H142" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
     <row r="143" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="144" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="145" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>

</xml_diff>

<commit_message>
bert and glove updated
</commit_message>
<xml_diff>
--- a/Keyword Map NLP.xlsx
+++ b/Keyword Map NLP.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="153">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="156">
   <si>
     <t xml:space="preserve">Keyword</t>
   </si>
@@ -130,355 +130,364 @@
     <t xml:space="preserve">kitchen</t>
   </si>
   <si>
+    <t xml:space="preserve">livingroom</t>
+  </si>
+  <si>
+    <t xml:space="preserve">bedroom</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dining</t>
+  </si>
+  <si>
+    <t xml:space="preserve">bathroom</t>
+  </si>
+  <si>
+    <t xml:space="preserve">basement</t>
+  </si>
+  <si>
+    <t xml:space="preserve">laundry</t>
+  </si>
+  <si>
+    <t xml:space="preserve">attic</t>
+  </si>
+  <si>
+    <t xml:space="preserve">den</t>
+  </si>
+  <si>
+    <t xml:space="preserve">hallway</t>
+  </si>
+  <si>
+    <t xml:space="preserve">garage</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sunroom</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pantry</t>
+  </si>
+  <si>
+    <t xml:space="preserve">closet</t>
+  </si>
+  <si>
+    <t xml:space="preserve">parlor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">entryway</t>
+  </si>
+  <si>
+    <t xml:space="preserve">lobby</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cellar</t>
+  </si>
+  <si>
+    <t xml:space="preserve">loft</t>
+  </si>
+  <si>
+    <t xml:space="preserve">nursery</t>
+  </si>
+  <si>
+    <t xml:space="preserve">coffee</t>
+  </si>
+  <si>
+    <t xml:space="preserve">food</t>
+  </si>
+  <si>
+    <t xml:space="preserve">washer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dryer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">stove</t>
+  </si>
+  <si>
+    <t xml:space="preserve">oven</t>
+  </si>
+  <si>
+    <t xml:space="preserve">microwave</t>
+  </si>
+  <si>
+    <t xml:space="preserve">spoon</t>
+  </si>
+  <si>
+    <t xml:space="preserve">fork</t>
+  </si>
+  <si>
+    <t xml:space="preserve">knife</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sofa</t>
+  </si>
+  <si>
+    <t xml:space="preserve">couch</t>
+  </si>
+  <si>
+    <t xml:space="preserve">television</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pillow</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sheets</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dresser</t>
+  </si>
+  <si>
+    <t xml:space="preserve">clothes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">shirt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pants</t>
+  </si>
+  <si>
+    <t xml:space="preserve">shorts</t>
+  </si>
+  <si>
+    <t xml:space="preserve">shoes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">socks</t>
+  </si>
+  <si>
+    <t xml:space="preserve">hat</t>
+  </si>
+  <si>
+    <t xml:space="preserve">toilet</t>
+  </si>
+  <si>
+    <t xml:space="preserve">toothbrush</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sink</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pot</t>
+  </si>
+  <si>
+    <t xml:space="preserve">shower</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mirror</t>
+  </si>
+  <si>
+    <t xml:space="preserve">phone</t>
+  </si>
+  <si>
+    <t xml:space="preserve">glass</t>
+  </si>
+  <si>
+    <t xml:space="preserve">drawer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">refrigerator</t>
+  </si>
+  <si>
+    <t xml:space="preserve">fan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">table</t>
+  </si>
+  <si>
+    <t xml:space="preserve">chair</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pet</t>
+  </si>
+  <si>
+    <t xml:space="preserve">meal</t>
+  </si>
+  <si>
+    <t xml:space="preserve">breakfast</t>
+  </si>
+  <si>
+    <t xml:space="preserve">lunch</t>
+  </si>
+  <si>
+    <t xml:space="preserve">super </t>
+  </si>
+  <si>
+    <t xml:space="preserve">dinner</t>
+  </si>
+  <si>
+    <t xml:space="preserve">fruit</t>
+  </si>
+  <si>
+    <t xml:space="preserve">vegetable</t>
+  </si>
+  <si>
+    <t xml:space="preserve">meat</t>
+  </si>
+  <si>
+    <t xml:space="preserve">yes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">correct</t>
+  </si>
+  <si>
+    <t xml:space="preserve">positive</t>
+  </si>
+  <si>
+    <t xml:space="preserve">agreed</t>
+  </si>
+  <si>
+    <t xml:space="preserve">disagree</t>
+  </si>
+  <si>
+    <t xml:space="preserve">no</t>
+  </si>
+  <si>
+    <t xml:space="preserve">negative</t>
+  </si>
+  <si>
+    <t xml:space="preserve">incorrect</t>
+  </si>
+  <si>
+    <t xml:space="preserve">listen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">play</t>
+  </si>
+  <si>
+    <t xml:space="preserve">open</t>
+  </si>
+  <si>
+    <t xml:space="preserve">close</t>
+  </si>
+  <si>
+    <t xml:space="preserve">wash</t>
+  </si>
+  <si>
+    <t xml:space="preserve">bathe</t>
+  </si>
+  <si>
+    <t xml:space="preserve">wait</t>
+  </si>
+  <si>
+    <t xml:space="preserve">watch</t>
+  </si>
+  <si>
+    <t xml:space="preserve">run</t>
+  </si>
+  <si>
+    <t xml:space="preserve">use</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dispose</t>
+  </si>
+  <si>
+    <t xml:space="preserve">throw away</t>
+  </si>
+  <si>
+    <t xml:space="preserve">trash</t>
+  </si>
+  <si>
+    <t xml:space="preserve">take out</t>
+  </si>
+  <si>
+    <t xml:space="preserve">thaw</t>
+  </si>
+  <si>
+    <t xml:space="preserve">create</t>
+  </si>
+  <si>
+    <t xml:space="preserve">prepare</t>
+  </si>
+  <si>
+    <t xml:space="preserve">turn off</t>
+  </si>
+  <si>
+    <t xml:space="preserve">turn on</t>
+  </si>
+  <si>
+    <t xml:space="preserve">find</t>
+  </si>
+  <si>
+    <t xml:space="preserve">discover</t>
+  </si>
+  <si>
+    <t xml:space="preserve">start</t>
+  </si>
+  <si>
+    <t xml:space="preserve">hello</t>
+  </si>
+  <si>
+    <t xml:space="preserve">where</t>
+  </si>
+  <si>
+    <t xml:space="preserve">what</t>
+  </si>
+  <si>
+    <t xml:space="preserve">am</t>
+  </si>
+  <si>
+    <t xml:space="preserve">here</t>
+  </si>
+  <si>
+    <t xml:space="preserve">camera</t>
+  </si>
+  <si>
+    <t xml:space="preserve">app</t>
+  </si>
+  <si>
+    <t xml:space="preserve">shut</t>
+  </si>
+  <si>
+    <t xml:space="preserve">shutdown</t>
+  </si>
+  <si>
+    <t xml:space="preserve">restart</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pause</t>
+  </si>
+  <si>
+    <t xml:space="preserve">resume</t>
+  </si>
+  <si>
+    <t xml:space="preserve">skip</t>
+  </si>
+  <si>
+    <t xml:space="preserve">video</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rewind</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cabinet</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ottoman</t>
+  </si>
+  <si>
+    <t xml:space="preserve">bookcase</t>
+  </si>
+  <si>
+    <t xml:space="preserve">futon</t>
+  </si>
+  <si>
+    <t xml:space="preserve">stool</t>
+  </si>
+  <si>
+    <t xml:space="preserve">nightstand</t>
+  </si>
+  <si>
+    <t xml:space="preserve">bench</t>
+  </si>
+  <si>
+    <t xml:space="preserve">room</t>
+  </si>
+  <si>
+    <t xml:space="preserve">living</t>
+  </si>
+  <si>
     <t xml:space="preserve">living room</t>
-  </si>
-  <si>
-    <t xml:space="preserve">bedroom</t>
-  </si>
-  <si>
-    <t xml:space="preserve">dining room</t>
-  </si>
-  <si>
-    <t xml:space="preserve">bathroom</t>
-  </si>
-  <si>
-    <t xml:space="preserve">basement</t>
-  </si>
-  <si>
-    <t xml:space="preserve">laundry room</t>
-  </si>
-  <si>
-    <t xml:space="preserve">attic</t>
-  </si>
-  <si>
-    <t xml:space="preserve">den</t>
-  </si>
-  <si>
-    <t xml:space="preserve">hallway</t>
-  </si>
-  <si>
-    <t xml:space="preserve">garage</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sunroom</t>
-  </si>
-  <si>
-    <t xml:space="preserve">pantry</t>
-  </si>
-  <si>
-    <t xml:space="preserve">closet</t>
-  </si>
-  <si>
-    <t xml:space="preserve">parlor</t>
-  </si>
-  <si>
-    <t xml:space="preserve">entryway</t>
-  </si>
-  <si>
-    <t xml:space="preserve">lobby</t>
-  </si>
-  <si>
-    <t xml:space="preserve">cellar</t>
-  </si>
-  <si>
-    <t xml:space="preserve">loft</t>
-  </si>
-  <si>
-    <t xml:space="preserve">nursery</t>
-  </si>
-  <si>
-    <t xml:space="preserve">coffee</t>
-  </si>
-  <si>
-    <t xml:space="preserve">food</t>
-  </si>
-  <si>
-    <t xml:space="preserve">washer</t>
-  </si>
-  <si>
-    <t xml:space="preserve">dryer</t>
-  </si>
-  <si>
-    <t xml:space="preserve">stove</t>
-  </si>
-  <si>
-    <t xml:space="preserve">oven</t>
-  </si>
-  <si>
-    <t xml:space="preserve">microwave</t>
-  </si>
-  <si>
-    <t xml:space="preserve">spoon</t>
-  </si>
-  <si>
-    <t xml:space="preserve">fork</t>
-  </si>
-  <si>
-    <t xml:space="preserve">knife</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sofa</t>
-  </si>
-  <si>
-    <t xml:space="preserve">couch</t>
-  </si>
-  <si>
-    <t xml:space="preserve">television</t>
-  </si>
-  <si>
-    <t xml:space="preserve">pillow</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sheets</t>
-  </si>
-  <si>
-    <t xml:space="preserve">dresser</t>
-  </si>
-  <si>
-    <t xml:space="preserve">clothes</t>
-  </si>
-  <si>
-    <t xml:space="preserve">shirt</t>
-  </si>
-  <si>
-    <t xml:space="preserve">pants</t>
-  </si>
-  <si>
-    <t xml:space="preserve">shorts</t>
-  </si>
-  <si>
-    <t xml:space="preserve">shoes</t>
-  </si>
-  <si>
-    <t xml:space="preserve">socks</t>
-  </si>
-  <si>
-    <t xml:space="preserve">hat</t>
-  </si>
-  <si>
-    <t xml:space="preserve">toilet</t>
-  </si>
-  <si>
-    <t xml:space="preserve">toothbrush</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sink</t>
-  </si>
-  <si>
-    <t xml:space="preserve">pot</t>
-  </si>
-  <si>
-    <t xml:space="preserve">shower</t>
-  </si>
-  <si>
-    <t xml:space="preserve">mirror</t>
-  </si>
-  <si>
-    <t xml:space="preserve">phone</t>
-  </si>
-  <si>
-    <t xml:space="preserve">glass</t>
-  </si>
-  <si>
-    <t xml:space="preserve">drawer</t>
-  </si>
-  <si>
-    <t xml:space="preserve">refrigerator</t>
-  </si>
-  <si>
-    <t xml:space="preserve">fan</t>
-  </si>
-  <si>
-    <t xml:space="preserve">AC</t>
-  </si>
-  <si>
-    <t xml:space="preserve">table</t>
-  </si>
-  <si>
-    <t xml:space="preserve">chair</t>
-  </si>
-  <si>
-    <t xml:space="preserve">pet</t>
-  </si>
-  <si>
-    <t xml:space="preserve">meal</t>
-  </si>
-  <si>
-    <t xml:space="preserve">breakfast</t>
-  </si>
-  <si>
-    <t xml:space="preserve">lunch</t>
-  </si>
-  <si>
-    <t xml:space="preserve">super </t>
-  </si>
-  <si>
-    <t xml:space="preserve">dinner</t>
-  </si>
-  <si>
-    <t xml:space="preserve">fruit</t>
-  </si>
-  <si>
-    <t xml:space="preserve">vegetable</t>
-  </si>
-  <si>
-    <t xml:space="preserve">meat</t>
-  </si>
-  <si>
-    <t xml:space="preserve">yes</t>
-  </si>
-  <si>
-    <t xml:space="preserve">correct</t>
-  </si>
-  <si>
-    <t xml:space="preserve">positive</t>
-  </si>
-  <si>
-    <t xml:space="preserve">agreed</t>
-  </si>
-  <si>
-    <t xml:space="preserve">disagree</t>
-  </si>
-  <si>
-    <t xml:space="preserve">no</t>
-  </si>
-  <si>
-    <t xml:space="preserve">negative</t>
-  </si>
-  <si>
-    <t xml:space="preserve">incorrect</t>
-  </si>
-  <si>
-    <t xml:space="preserve">listen</t>
-  </si>
-  <si>
-    <t xml:space="preserve">play</t>
-  </si>
-  <si>
-    <t xml:space="preserve">open</t>
-  </si>
-  <si>
-    <t xml:space="preserve">close</t>
-  </si>
-  <si>
-    <t xml:space="preserve">wash</t>
-  </si>
-  <si>
-    <t xml:space="preserve">bathe</t>
-  </si>
-  <si>
-    <t xml:space="preserve">wait</t>
-  </si>
-  <si>
-    <t xml:space="preserve">watch</t>
-  </si>
-  <si>
-    <t xml:space="preserve">run</t>
-  </si>
-  <si>
-    <t xml:space="preserve">use</t>
-  </si>
-  <si>
-    <t xml:space="preserve">dispose</t>
-  </si>
-  <si>
-    <t xml:space="preserve">throw away</t>
-  </si>
-  <si>
-    <t xml:space="preserve">trash</t>
-  </si>
-  <si>
-    <t xml:space="preserve">take out</t>
-  </si>
-  <si>
-    <t xml:space="preserve">thaw</t>
-  </si>
-  <si>
-    <t xml:space="preserve">create</t>
-  </si>
-  <si>
-    <t xml:space="preserve">prepare</t>
-  </si>
-  <si>
-    <t xml:space="preserve">turn off</t>
-  </si>
-  <si>
-    <t xml:space="preserve">turn on</t>
-  </si>
-  <si>
-    <t xml:space="preserve">find</t>
-  </si>
-  <si>
-    <t xml:space="preserve">discover</t>
-  </si>
-  <si>
-    <t xml:space="preserve">start</t>
-  </si>
-  <si>
-    <t xml:space="preserve">hello</t>
-  </si>
-  <si>
-    <t xml:space="preserve">where</t>
-  </si>
-  <si>
-    <t xml:space="preserve">what</t>
-  </si>
-  <si>
-    <t xml:space="preserve">am</t>
-  </si>
-  <si>
-    <t xml:space="preserve">here</t>
-  </si>
-  <si>
-    <t xml:space="preserve">camera</t>
-  </si>
-  <si>
-    <t xml:space="preserve">app</t>
-  </si>
-  <si>
-    <t xml:space="preserve">shut</t>
-  </si>
-  <si>
-    <t xml:space="preserve">shutdown</t>
-  </si>
-  <si>
-    <t xml:space="preserve">restart</t>
-  </si>
-  <si>
-    <t xml:space="preserve">pause</t>
-  </si>
-  <si>
-    <t xml:space="preserve">resume</t>
-  </si>
-  <si>
-    <t xml:space="preserve">skip</t>
-  </si>
-  <si>
-    <t xml:space="preserve">video</t>
-  </si>
-  <si>
-    <t xml:space="preserve">rewind</t>
-  </si>
-  <si>
-    <t xml:space="preserve">cabinet</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ottoman</t>
-  </si>
-  <si>
-    <t xml:space="preserve">bookcase</t>
-  </si>
-  <si>
-    <t xml:space="preserve">futon</t>
-  </si>
-  <si>
-    <t xml:space="preserve">stool</t>
-  </si>
-  <si>
-    <t xml:space="preserve">nightstand</t>
-  </si>
-  <si>
-    <t xml:space="preserve">bench</t>
   </si>
 </sst>
 </file>
@@ -586,11 +595,11 @@
   </sheetPr>
   <dimension ref="A1:H1024"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A94" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H157" activeCellId="0" sqref="H157"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A88" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="M132" activeCellId="0" sqref="M132"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.48046875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.49609375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="12.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="2" style="0" width="8.7"/>
@@ -4470,9 +4479,84 @@
         <v>0</v>
       </c>
     </row>
-    <row r="150" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="151" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="152" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="150" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A150" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="B150" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="C150" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="D150" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="E150" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="F150" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="G150" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="H150" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="151" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A151" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="B151" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="C151" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="D151" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="E151" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="F151" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="G151" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="H151" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="152" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A152" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="B152" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="C152" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="D152" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="E152" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="F152" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="G152" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="H152" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
     <row r="153" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="154" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="155" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>

</xml_diff>